<commit_message>
Getting Xpath of earnings to work
Delete extra stuff
</commit_message>
<xml_diff>
--- a/Copy of Updated-  StockExcelDesign - BNOEDIT (003).xlsx
+++ b/Copy of Updated-  StockExcelDesign - BNOEDIT (003).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aanker\Desktop\Stock_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EAAA770C-ABDD-450F-B62F-66ABB4866D75}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BDE8CD47-FFB0-4F3E-ADD5-C002B83EB1AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="8085" tabRatio="588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8085" tabRatio="588" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_2_2018 Stock List" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
   <si>
     <t>TWTR</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>IFNEEDED</t>
+  </si>
+  <si>
+    <t>&lt;--- REAL</t>
   </si>
 </sst>
 </file>
@@ -594,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,7 +1979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CT4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2411,10 +2417,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB60AEFA-EE82-48A1-8D46-3702A9F7DB94}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,7 +2579,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
         <v>46</v>
@@ -2583,7 +2589,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8" t="s">
         <v>47</v>
@@ -2593,7 +2599,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8" t="s">
         <v>48</v>
@@ -2603,7 +2609,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8" t="s">
         <v>49</v>
@@ -2613,7 +2619,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>28</v>
       </c>
@@ -2624,8 +2630,11 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
@@ -2641,7 +2650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8" t="s">
         <v>32</v>
@@ -2651,7 +2660,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8" t="s">
         <v>33</v>
@@ -2661,7 +2670,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8" t="s">
         <v>34</v>
@@ -2671,7 +2680,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8" t="s">
         <v>35</v>
@@ -2681,125 +2690,304 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
-      <c r="B27" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="B30" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-      <c r="C34" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>